<commit_message>
Fixes to the Documentation
</commit_message>
<xml_diff>
--- a/Sprint 3 Agility Gantt Chart.xlsx
+++ b/Sprint 3 Agility Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pilotmania/Desktop/OneDrive - Monmouth University/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pilotmania/Documents/GitHub/CS104-Sprint-3-Agility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57D06BDB-E39D-4A4F-A22C-625BA9606A74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6CFE80-9722-B34C-B1F2-2874AE7C9ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32940" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1082,7 +1082,7 @@
   <dimension ref="B1:BP30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>